<commit_message>
committing some changes to add_top3 and clean prio + indenting
</commit_message>
<xml_diff>
--- a/resources/hesper_key.xlsx
+++ b/resources/hesper_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted.sharepoint.com/sites/IMPACTHQ-Accountability&amp;Inclusion/Documents partages/General/12_Accountability to Affected People Specialist/07_Hesper Scale/5. Standard tool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/raphael_bacot_impact-initiatives_org/Documents/git/hespeR/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="706" documentId="8_{7CACD3A7-BA64-4CBF-8FCB-2196D69A14AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6DE3F7A-5B7F-4770-9007-F6C66FEAB00E}"/>
+  <xr:revisionPtr revIDLastSave="710" documentId="8_{7CACD3A7-BA64-4CBF-8FCB-2196D69A14AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE2B838D-B921-49D8-AACE-15E67A9DF5AA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B423C696-7984-4BF5-9643-B9D359E34A33}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B423C696-7984-4BF5-9643-B9D359E34A33}"/>
   </bookViews>
   <sheets>
     <sheet name="key" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2602" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2602" uniqueCount="481">
   <si>
     <t>H1_hesper_drinking_water</t>
   </si>
@@ -1312,15 +1312,6 @@
     <t>name_ind</t>
   </si>
   <si>
-    <t>hesper_clean_men</t>
-  </si>
-  <si>
-    <t>women</t>
-  </si>
-  <si>
-    <t>men</t>
-  </si>
-  <si>
     <t>distress</t>
   </si>
   <si>
@@ -1484,6 +1475,18 @@
   </si>
   <si>
     <t>Mental health issues in your community</t>
+  </si>
+  <si>
+    <t>hesper_health_care_male</t>
+  </si>
+  <si>
+    <t>hesper_health_care_female</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>male</t>
   </si>
 </sst>
 </file>
@@ -1891,8 +1894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F9C564-72CF-48CA-9D8B-89F7531192AA}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1910,19 +1913,19 @@
         <v>223</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>428</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>431</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>147</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>421</v>
@@ -1988,10 +1991,10 @@
         <v>171</v>
       </c>
       <c r="J2" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="K2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>153</v>
@@ -2026,7 +2029,7 @@
         <v>371</v>
       </c>
       <c r="E3" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
@@ -2042,10 +2045,10 @@
         <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="K3" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>153</v>
@@ -2080,7 +2083,7 @@
         <v>372</v>
       </c>
       <c r="E4" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="F4" t="s">
         <v>38</v>
@@ -2096,10 +2099,10 @@
         <v>38</v>
       </c>
       <c r="J4" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="K4" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>153</v>
@@ -2134,7 +2137,7 @@
         <v>373</v>
       </c>
       <c r="E5" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F5" t="s">
         <v>172</v>
@@ -2150,10 +2153,10 @@
         <v>172</v>
       </c>
       <c r="J5" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="K5" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>153</v>
@@ -2182,19 +2185,19 @@
         <v>268</v>
       </c>
       <c r="C6" t="s">
-        <v>424</v>
+        <v>480</v>
       </c>
       <c r="D6" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E6" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="F6" t="s">
         <v>403</v>
       </c>
       <c r="G6" t="s">
-        <v>422</v>
+        <v>173</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -2204,10 +2207,10 @@
         <v>403</v>
       </c>
       <c r="J6" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="K6" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>153</v>
@@ -2233,35 +2236,35 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>423</v>
+        <v>479</v>
       </c>
       <c r="C7" t="s">
-        <v>423</v>
+        <v>479</v>
       </c>
       <c r="D7" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E7" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="F7" t="s">
-        <v>404</v>
+        <v>174</v>
       </c>
       <c r="G7" t="s">
-        <v>404</v>
+        <v>174</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>hesper_top_three_priorities.hesper_clean_women</v>
+        <v>hesper_top_three_priorities.hesper_clean_female</v>
       </c>
       <c r="I7" t="s">
-        <v>404</v>
+        <v>174</v>
       </c>
       <c r="J7" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="K7" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>153</v>
@@ -2312,10 +2315,10 @@
         <v>175</v>
       </c>
       <c r="J8" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="K8" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>153</v>
@@ -2366,10 +2369,10 @@
         <v>176</v>
       </c>
       <c r="J9" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="K9" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>165</v>
@@ -2401,10 +2404,10 @@
         <v>268</v>
       </c>
       <c r="D10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E10" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="F10" t="s">
         <v>55</v>
@@ -2420,10 +2423,10 @@
         <v>55</v>
       </c>
       <c r="J10" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="K10" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>153</v>
@@ -2452,32 +2455,32 @@
         <v>268</v>
       </c>
       <c r="C11" t="s">
-        <v>424</v>
+        <v>480</v>
       </c>
       <c r="D11" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="E11" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="F11" t="s">
-        <v>405</v>
+        <v>477</v>
       </c>
       <c r="G11" t="s">
-        <v>405</v>
+        <v>477</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>hesper_top_three_priorities.hesper_health_care_men</v>
+        <v>hesper_top_three_priorities.hesper_health_care_male</v>
       </c>
       <c r="I11" t="s">
-        <v>405</v>
+        <v>477</v>
       </c>
       <c r="J11" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="K11" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>153</v>
@@ -2506,32 +2509,32 @@
         <v>268</v>
       </c>
       <c r="C12" t="s">
-        <v>423</v>
+        <v>479</v>
       </c>
       <c r="D12" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="E12" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="F12" t="s">
-        <v>406</v>
+        <v>478</v>
       </c>
       <c r="G12" t="s">
-        <v>406</v>
+        <v>478</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>hesper_top_three_priorities.hesper_health_care_women</v>
+        <v>hesper_top_three_priorities.hesper_health_care_female</v>
       </c>
       <c r="I12" t="s">
-        <v>406</v>
+        <v>478</v>
       </c>
       <c r="J12" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="K12" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>153</v>
@@ -2582,10 +2585,10 @@
         <v>407</v>
       </c>
       <c r="J13" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="K13" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>157</v>
@@ -2620,7 +2623,7 @@
         <v>382</v>
       </c>
       <c r="E14" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F14" t="s">
         <v>180</v>
@@ -2636,10 +2639,10 @@
         <v>180</v>
       </c>
       <c r="J14" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="K14" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>157</v>
@@ -2674,7 +2677,7 @@
         <v>383</v>
       </c>
       <c r="E15" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="F15" t="s">
         <v>71</v>
@@ -2690,10 +2693,10 @@
         <v>71</v>
       </c>
       <c r="J15" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="K15" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>157</v>
@@ -2725,10 +2728,10 @@
         <v>268</v>
       </c>
       <c r="D16" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E16" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="F16" t="s">
         <v>181</v>
@@ -2744,10 +2747,10 @@
         <v>181</v>
       </c>
       <c r="J16" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="K16" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>157</v>
@@ -2798,10 +2801,10 @@
         <v>182</v>
       </c>
       <c r="J17" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="K17" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>157</v>
@@ -2836,7 +2839,7 @@
         <v>386</v>
       </c>
       <c r="E18" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="F18" t="s">
         <v>183</v>
@@ -2852,10 +2855,10 @@
         <v>183</v>
       </c>
       <c r="J18" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="K18" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>157</v>
@@ -2881,16 +2884,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C19" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D19" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E19" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="F19" t="s">
         <v>184</v>
@@ -2909,7 +2912,7 @@
         <v>168</v>
       </c>
       <c r="K19" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>157</v>
@@ -2941,10 +2944,10 @@
         <v>268</v>
       </c>
       <c r="D20" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E20" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F20" t="s">
         <v>88</v>
@@ -2960,10 +2963,10 @@
         <v>88</v>
       </c>
       <c r="J20" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="K20" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>157</v>
@@ -3017,7 +3020,7 @@
         <v>411</v>
       </c>
       <c r="K21" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>157</v>
@@ -3068,10 +3071,10 @@
         <v>94</v>
       </c>
       <c r="J22" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="K22" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>157</v>
@@ -3122,10 +3125,10 @@
         <v>98</v>
       </c>
       <c r="J23" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="K23" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>157</v>
@@ -3160,7 +3163,7 @@
         <v>393</v>
       </c>
       <c r="E24" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="F24" t="s">
         <v>188</v>
@@ -3176,10 +3179,10 @@
         <v>188</v>
       </c>
       <c r="J24" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="K24" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>157</v>
@@ -3356,10 +3359,10 @@
         <v>154</v>
       </c>
       <c r="P27" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="Q27" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
@@ -3373,10 +3376,10 @@
         <v>268</v>
       </c>
       <c r="D28" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E28" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="F28" t="s">
         <v>191</v>
@@ -3410,10 +3413,10 @@
         <v>155</v>
       </c>
       <c r="P28" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="Q28" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
@@ -3427,10 +3430,10 @@
         <v>268</v>
       </c>
       <c r="D29" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E29" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="F29" t="s">
         <v>192</v>
@@ -10954,6 +10957,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d0fa6634-326e-4532-91a2-52bea7ac9212" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f4877444-78fa-4cfa-bafc-d6c64fafc061">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DE51FB2AFBB2DD429D3D11FE759FFC43" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="aef6d84b9533c2c7e1fb337c73d9c69e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f4877444-78fa-4cfa-bafc-d6c64fafc061" xmlns:ns3="d0fa6634-326e-4532-91a2-52bea7ac9212" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cc3ba5565c046c17d5dfc9699468446" ns2:_="" ns3:_="">
     <xsd:import namespace="f4877444-78fa-4cfa-bafc-d6c64fafc061"/>
@@ -11182,27 +11205,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d0fa6634-326e-4532-91a2-52bea7ac9212" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f4877444-78fa-4cfa-bafc-d6c64fafc061">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B45EED0F-3E73-4158-A37E-474D1AB3BE58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{470AF310-420B-4274-B284-07FB9965998A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d0fa6634-326e-4532-91a2-52bea7ac9212"/>
+    <ds:schemaRef ds:uri="f4877444-78fa-4cfa-bafc-d6c64fafc061"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F06CA42D-342D-48D8-9E95-C92FAF8A9450}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11219,23 +11241,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{470AF310-420B-4274-B284-07FB9965998A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d0fa6634-326e-4532-91a2-52bea7ac9212"/>
-    <ds:schemaRef ds:uri="f4877444-78fa-4cfa-bafc-d6c64fafc061"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B45EED0F-3E73-4158-A37E-474D1AB3BE58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add draft script to align dataset to standard package values
</commit_message>
<xml_diff>
--- a/resources/hesper_key.xlsx
+++ b/resources/hesper_key.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="710" documentId="8_{7CACD3A7-BA64-4CBF-8FCB-2196D69A14AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE2B838D-B921-49D8-AACE-15E67A9DF5AA}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B423C696-7984-4BF5-9643-B9D359E34A33}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B423C696-7984-4BF5-9643-B9D359E34A33}"/>
   </bookViews>
   <sheets>
     <sheet name="key" sheetId="3" r:id="rId1"/>
@@ -1895,7 +1895,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10957,26 +10957,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d0fa6634-326e-4532-91a2-52bea7ac9212" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f4877444-78fa-4cfa-bafc-d6c64fafc061">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DE51FB2AFBB2DD429D3D11FE759FFC43" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="aef6d84b9533c2c7e1fb337c73d9c69e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f4877444-78fa-4cfa-bafc-d6c64fafc061" xmlns:ns3="d0fa6634-326e-4532-91a2-52bea7ac9212" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4cc3ba5565c046c17d5dfc9699468446" ns2:_="" ns3:_="">
     <xsd:import namespace="f4877444-78fa-4cfa-bafc-d6c64fafc061"/>
@@ -11205,10 +11185,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d0fa6634-326e-4532-91a2-52bea7ac9212" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f4877444-78fa-4cfa-bafc-d6c64fafc061">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B45EED0F-3E73-4158-A37E-474D1AB3BE58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F06CA42D-342D-48D8-9E95-C92FAF8A9450}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f4877444-78fa-4cfa-bafc-d6c64fafc061"/>
+    <ds:schemaRef ds:uri="d0fa6634-326e-4532-91a2-52bea7ac9212"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11225,20 +11236,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F06CA42D-342D-48D8-9E95-C92FAF8A9450}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B45EED0F-3E73-4158-A37E-474D1AB3BE58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f4877444-78fa-4cfa-bafc-d6c64fafc061"/>
-    <ds:schemaRef ds:uri="d0fa6634-326e-4532-91a2-52bea7ac9212"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>